<commit_message>
feat: :sparkles: novos scrapings
</commit_message>
<xml_diff>
--- a/imoveis.xlsx
+++ b/imoveis.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Título</t>
   </si>
@@ -23,93 +23,6 @@
   </si>
   <si>
     <t>Detalhes</t>
-  </si>
-  <si>
-    <t>Casas à venda no Villas Ohana | Tamandaré-PE</t>
-  </si>
-  <si>
-    <t>R$995.300,00</t>
-  </si>
-  <si>
-    <t>VENDA</t>
-  </si>
-  <si>
-    <t>3 Dormitórios, sendo 1 suíte, 3 Banheiros, 1 Cozinha, 1 Sala de estar, 1 Área de serviço</t>
-  </si>
-  <si>
-    <t>Apartamentos à venda no Açores Tamandaré Flats</t>
-  </si>
-  <si>
-    <t>R$260.000,00</t>
-  </si>
-  <si>
-    <t>1 Dormitório, 1 Banheiro, 1 Cozinha</t>
-  </si>
-  <si>
-    <t>Casa de alto pdrão à venda no Condomínio Terras Alpha | Caruaru-PE</t>
-  </si>
-  <si>
-    <t>R$1.500.000,00</t>
-  </si>
-  <si>
-    <t>4 Dormitórios, sendo 4 suítes, 5 Banheiros, 4 Garagens, 1 Closet, 1 Copa, 1 Cozinha, 1 Lavabo, 1 Sala de jantar, 1 Sala de estar, 1 Área de serviço, 1 Dependência p/empregada</t>
-  </si>
-  <si>
-    <t>Casa de alto padrão à venda no Condomínio Terras Alpha | Caruaru-PE</t>
-  </si>
-  <si>
-    <t>R$1.450.000,00</t>
-  </si>
-  <si>
-    <t>R$1.150.000,00</t>
-  </si>
-  <si>
-    <t>4 Dormitórios, sendo 3 suítes, 5 Banheiros, 4 Garagens, 3 Closets, 1 Copa, 1 Cozinha, 2 Lavabos, 1 Sala de jantar, 1 Sala de estar, 1 Área de serviço, 1 Dependência p/empregada</t>
-  </si>
-  <si>
-    <t>Casas à venda no Bairro Luiz Gonzaga | Caruaru-PE</t>
-  </si>
-  <si>
-    <t>R$530.000,00</t>
-  </si>
-  <si>
-    <t>3 Dormitórios, 1 Banheiro, 2 Garagens, 1 Closet, 1 Cozinha, 1 Sala de jantar, 1 Sala de estar, 1 Área de serviço</t>
-  </si>
-  <si>
-    <t>Casa à venda no Bairro Luiz Gonzaga | Caruaru-PE</t>
-  </si>
-  <si>
-    <t>R$390.000,00</t>
-  </si>
-  <si>
-    <t>4 Dormitórios, sendo 1 suíte, 2 Banheiros, 2 Garagens, 1 Closet, 1 Escritório, 1 Sala de TV, 1 Cozinha, 1 Sala de jantar, 1 Sala de estar, 1 Área de serviço</t>
-  </si>
-  <si>
-    <t>Casas Duplex à venda no One Residence | Maurício de Nassau</t>
-  </si>
-  <si>
-    <t>R$799.000,00</t>
-  </si>
-  <si>
-    <t>4 Dormitórios, sendo 4 suítes, 5 Banheiros, 3 Garagens, 4 Closets, 1 Cozinha, 1 Sala de jantar, 1 Sala de estar, 1 Área de serviço</t>
-  </si>
-  <si>
-    <t>Terreno à venda no Condomínio Quintas da Colina 1 | Caruaru-PE</t>
-  </si>
-  <si>
-    <t>R$520.000,00</t>
-  </si>
-  <si>
-    <t>Churrasqueira, Interfone, Piscina infantil, Playground, Portaria 24 horas, Portão Elétrico, Quadra poliesportiva, Ronda motorizada, Sala de jogos, Salão de festas, Sauna, Área verde preservada</t>
-  </si>
-  <si>
-    <t>Casa à venda no Bairro Vila Kennedy | Caruaru-PE</t>
-  </si>
-  <si>
-    <t>R$320.000,00</t>
-  </si>
-  <si>
-    <t>3 Dormitórios, sendo 1 suíte, 2 Banheiros, 2 Garagens, 1 Cozinha, 1 Sala de jantar, 1 Sala de estar, 1 Área de serviço</t>
   </si>
 </sst>
 </file>
@@ -486,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -508,146 +421,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>